<commit_message>
excelsheet upload for ITAssset,Employee,NonITAsset
</commit_message>
<xml_diff>
--- a/AppFiles/Images/Logo/EmployeeBulkUploadTemplate.xlsx
+++ b/AppFiles/Images/Logo/EmployeeBulkUploadTemplate.xlsx
@@ -62,12 +62,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0;[Red]0"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -110,9 +111,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -125,6 +125,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -133,8 +154,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,91 +200,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,11 +224,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -263,13 +264,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,13 +306,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,43 +432,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,97 +444,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,21 +455,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -513,6 +499,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -535,13 +532,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,164 +558,164 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -979,8 +980,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -7045,11 +7046,11 @@
     <dataValidation type="list" allowBlank="1" sqref="E2:E1000">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" sqref="M2:M1000">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(M2))),AND(ISNUMBER(M2),LEFT(CELL("format",M2))="D"))</formula1>
+    </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" sqref="N2:N1000">
       <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" sqref="M2:M1000">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(M2))),AND(ISNUMBER(M2),LEFT(CELL("format",M2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Upload excel in Consumables
</commit_message>
<xml_diff>
--- a/AppFiles/Images/Logo/EmployeeBulkUploadTemplate.xlsx
+++ b/AppFiles/Images/Logo/EmployeeBulkUploadTemplate.xlsx
@@ -64,11 +64,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="dd/mmm/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd\/mmm\/yyyy;@"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -112,7 +112,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -132,8 +140,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,16 +163,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,33 +193,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,32 +211,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,6 +232,28 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -264,7 +264,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,13 +378,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +408,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,115 +426,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,13 +444,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,6 +482,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -508,11 +517,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,21 +547,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -558,148 +558,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -980,8 +980,8 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>